<commit_message>
SERPM 2040 Test Network (not sure if it worked)
Regional model zone system with 4500 zones is being tested.. There seems to be some issue with the network that led to crash after first iteration.
</commit_message>
<xml_diff>
--- a/Input_Fields.xlsx
+++ b/Input_Fields.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
   <si>
     <t>A</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>LENGTH</t>
+  </si>
+  <si>
+    <t>FTC2</t>
   </si>
 </sst>
 </file>
@@ -298,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -312,6 +315,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46E1AC0-A8E3-4714-8F2B-DFF4DA726E14}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +643,7 @@
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>24</v>
       </c>
@@ -650,7 +654,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -660,8 +664,11 @@
       <c r="C2" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -671,8 +678,11 @@
       <c r="C3" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -682,8 +692,11 @@
       <c r="C4" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -693,8 +706,11 @@
       <c r="C5" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
@@ -704,8 +720,11 @@
       <c r="C6" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -715,8 +734,11 @@
       <c r="C7" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -726,8 +748,11 @@
       <c r="C8" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -737,30 +762,36 @@
       <c r="C9" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
@@ -771,7 +802,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>22</v>
       </c>
@@ -782,7 +813,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>26</v>
       </c>

</xml_diff>